<commit_message>
changes made for US demo - Manual insights
</commit_message>
<xml_diff>
--- a/campaigns.xlsx
+++ b/campaigns.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://zendatashastra01-my.sharepoint.com/personal/sunil_zendatashastra_com/Documents/Clients/ZDS/CampAIgn_PydanticAI/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="11_625DE4A3144642BE6D7D38955A5DCE3A8746195F" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5BB6336D-7C80-490E-B1A5-29953D60FD99}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="11_625DE4A3144642BE6D7D38955A5DCE3A8746195F" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5EA76B49-846A-4D07-AEA4-73985C5D4502}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="32220" yWindow="3420" windowWidth="21600" windowHeight="11175" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1310,10 +1310,29 @@
   <dimension ref="A1:Q101"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection sqref="A1:Q1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="16.08984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.36328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.36328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.36328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.90625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.453125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.54296875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.6328125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.1796875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20.54296875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.7265625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="17.26953125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="17.1796875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="19.36328125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="15.81640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="14.453125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">

</xml_diff>